<commit_message>
Finished scrapper for all sheets
</commit_message>
<xml_diff>
--- a/HK_2021.xlsx
+++ b/HK_2021.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12330" tabRatio="600" firstSheet="1" activeTab="2" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12330" tabRatio="600" firstSheet="1" activeTab="3" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="服務收費" sheetId="1" state="hidden" r:id="rId1"/>
@@ -1159,14 +1159,14 @@
       <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="8.85546875" defaultRowHeight="15" outlineLevelCol="0"/>
   <cols>
     <col width="75.28515625" bestFit="1" customWidth="1" style="2" min="1" max="1"/>
     <col width="9.42578125" bestFit="1" customWidth="1" style="2" min="2" max="2"/>
     <col width="47.42578125" bestFit="1" customWidth="1" style="2" min="3" max="3"/>
     <col width="11.140625" bestFit="1" customWidth="1" style="2" min="4" max="4"/>
-    <col width="8.85546875" customWidth="1" style="2" min="5" max="15"/>
-    <col width="8.85546875" customWidth="1" style="2" min="16" max="16384"/>
+    <col width="8.85546875" customWidth="1" style="2" min="5" max="22"/>
+    <col width="8.85546875" customWidth="1" style="2" min="23" max="16384"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -1430,19 +1430,19 @@
   </sheetPr>
   <dimension ref="A1:E27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="8.85546875" defaultRowHeight="15" outlineLevelCol="0"/>
   <cols>
     <col width="16.140625" bestFit="1" customWidth="1" style="5" min="1" max="1"/>
     <col width="10.140625" bestFit="1" customWidth="1" style="5" min="2" max="2"/>
     <col width="9.7109375" bestFit="1" customWidth="1" style="5" min="3" max="3"/>
     <col width="9.42578125" bestFit="1" customWidth="1" style="5" min="4" max="4"/>
     <col width="10.7109375" bestFit="1" customWidth="1" style="5" min="5" max="5"/>
-    <col width="8.85546875" customWidth="1" style="5" min="6" max="16"/>
-    <col width="8.85546875" customWidth="1" style="5" min="17" max="16384"/>
+    <col width="8.85546875" customWidth="1" style="5" min="6" max="23"/>
+    <col width="8.85546875" customWidth="1" style="5" min="24" max="16384"/>
   </cols>
   <sheetData>
     <row r="1" ht="15.75" customHeight="1" s="19" thickBot="1">
@@ -1874,18 +1874,18 @@
   </sheetPr>
   <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L17" sqref="L17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="8.85546875" defaultRowHeight="15" outlineLevelCol="0"/>
   <cols>
     <col width="9.5703125" bestFit="1" customWidth="1" style="5" min="1" max="1"/>
     <col width="10.85546875" bestFit="1" customWidth="1" style="5" min="2" max="2"/>
     <col width="11.140625" bestFit="1" customWidth="1" style="5" min="3" max="4"/>
     <col width="10.28515625" bestFit="1" customWidth="1" style="5" min="5" max="5"/>
-    <col width="8.85546875" customWidth="1" style="5" min="6" max="16"/>
-    <col width="8.85546875" customWidth="1" style="5" min="17" max="16384"/>
+    <col width="8.85546875" customWidth="1" style="5" min="6" max="23"/>
+    <col width="8.85546875" customWidth="1" style="5" min="24" max="16384"/>
   </cols>
   <sheetData>
     <row r="1" ht="15.75" customHeight="1" s="19" thickBot="1">
@@ -2017,11 +2017,11 @@
       </c>
       <c r="B8" s="11" t="inlineStr">
         <is>
-          <t>600309.SH</t>
+          <t>600309.SS</t>
         </is>
       </c>
       <c r="C8" s="14" t="n">
-        <v/>
+        <v>118.9000015258789</v>
       </c>
       <c r="D8" s="11" t="n"/>
     </row>
@@ -2033,11 +2033,11 @@
       </c>
       <c r="B9" s="11" t="inlineStr">
         <is>
-          <t>600519.SH</t>
+          <t>600519.SS</t>
         </is>
       </c>
       <c r="C9" s="14" t="n">
-        <v/>
+        <v>1900</v>
       </c>
       <c r="D9" s="11" t="n"/>
     </row>
@@ -2062,18 +2062,18 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="8.85546875" defaultRowHeight="15" outlineLevelCol="0"/>
   <cols>
     <col width="23.7109375" bestFit="1" customWidth="1" style="5" min="1" max="1"/>
     <col width="13.7109375" bestFit="1" customWidth="1" style="5" min="2" max="2"/>
     <col width="9.28515625" bestFit="1" customWidth="1" style="5" min="3" max="3"/>
     <col width="11.85546875" bestFit="1" customWidth="1" style="5" min="4" max="4"/>
     <col width="8.7109375" bestFit="1" customWidth="1" style="5" min="5" max="5"/>
-    <col width="8.85546875" customWidth="1" style="5" min="6" max="16"/>
-    <col width="8.85546875" customWidth="1" style="5" min="17" max="16384"/>
+    <col width="8.85546875" customWidth="1" style="5" min="6" max="23"/>
+    <col width="8.85546875" customWidth="1" style="5" min="24" max="16384"/>
   </cols>
   <sheetData>
     <row r="1" ht="15.75" customHeight="1" s="19" thickBot="1">

</xml_diff>